<commit_message>
Upload stage 3 evidences B1-B2
</commit_message>
<xml_diff>
--- a/sarsersirsur/evidence.xlsx
+++ b/sarsersirsur/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\1W_sarsersirsur\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\0k_sarsersirsur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04800CBA-9DF1-4EB8-893E-C8560C49AE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179978D4-A331-4BA6-A893-A063A6B32864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="877" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="45">
   <si>
     <t>TxHash</t>
   </si>
@@ -167,6 +167,18 @@
   </si>
   <si>
     <t>6BF731557108FB609B2A5EBFA4EBFA4DECB3B1A3B013F6095E815DA756BCC6D3</t>
+  </si>
+  <si>
+    <t>FBFD588EDFD9275A1FFF4F141BA4827F83559F548168341C39EDAB0BB8E1241A</t>
+  </si>
+  <si>
+    <t>E331FC592E2A72E0D60590C5B767CE737AEB89E097AEDDF1FEBAF9DB2B2069DC</t>
+  </si>
+  <si>
+    <t>3161AEBB129ECB3D4A4E747DC5F1DA2EA4AA0FA3C7A4734D6454F82ABCBDB94A</t>
+  </si>
+  <si>
+    <t>8275A3624278481BA0F4161865AD61EBF95FB656CDF6B7E7D0BDB35C6D841237</t>
   </si>
 </sst>
 </file>
@@ -570,7 +582,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,6 +1226,78 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,7 +1310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1241,8 +1325,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1275,74 +1359,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
@@ -1559,7 +1575,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Upload evidences A7 to A20 and B5 to B7
</commit_message>
<xml_diff>
--- a/sarsersirsur/evidence.xlsx
+++ b/sarsersirsur/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\0k_sarsersirsur\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMUT\Desktop\coins\gon testnet\-_0k_sarsersirsur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179978D4-A331-4BA6-A893-A063A6B32864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D693CF6-1050-4824-99FC-C47DC19C1888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="877" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="877" firstSheet="3" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,47 +38,27 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="95">
   <si>
     <t>TxHash</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -179,13 +159,184 @@
   </si>
   <si>
     <t>8275A3624278481BA0F4161865AD61EBF95FB656CDF6B7E7D0BDB35C6D841237</t>
+  </si>
+  <si>
+    <t>ibc/B62340C438847FD0541E809B841D3D8A3498545C7DA15329A4E745CD30EE5F09</t>
+  </si>
+  <si>
+    <t>sarsersirsurA7</t>
+  </si>
+  <si>
+    <t>ibc/CA1629F5026ED1E6C2F3FEA07D509F7D5836747E5F921EECB6D16184077C4384</t>
+  </si>
+  <si>
+    <t>sarsersirsurA8</t>
+  </si>
+  <si>
+    <t>ibc/5B571645454832580E8B11B0145C3BEDD87AB941F60170AB74DE28E5B4DAA429</t>
+  </si>
+  <si>
+    <t>sarsersirsurA9</t>
+  </si>
+  <si>
+    <t>ibc/990648BB6D7976B00F75946E7EEB974FE57CC5E97893AD8FB08D751106ECDC52</t>
+  </si>
+  <si>
+    <t>sarsersirsurA10</t>
+  </si>
+  <si>
+    <t>ibc/BEAB83B560F7F9EFDF8570C2854E8C545B2E3EB9E4921EF2218602ED8B0A6A6B</t>
+  </si>
+  <si>
+    <t>sarsersirsurA11</t>
+  </si>
+  <si>
+    <t>ibc/1A4FAB4A430982FEFAB20A07C855EB03E4460750FED516B531DF3912D2F47517</t>
+  </si>
+  <si>
+    <t>sarsersirsurA12</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>FA67EA8DB76769A1B1BBCAA02C3721FC0B11E616EC067DC8B671BF4CDDFFC429</t>
+  </si>
+  <si>
+    <t>2EAF228793B0A818B4F28C84A86261EDC79478F14BE541D70F2566CB06E0EC4B</t>
+  </si>
+  <si>
+    <t>0A24C4F358091FF787BA512201C2905527BFAAF34D2026E621A23E89A43AD8E5</t>
+  </si>
+  <si>
+    <t>2FD349549CD030485E04C08900AC30FBAC1A5CC5F5975C8A9A557086DA5802F3</t>
+  </si>
+  <si>
+    <t>8D19C07946CD109AEB429A6E9864CAE098A668DA68D76F45E371658AF346F660</t>
+  </si>
+  <si>
+    <t>263A0EA66DE198F37E5D1985629B5AE767BF45B55F181FFA5BE68B611F4FAE7C</t>
+  </si>
+  <si>
+    <t>7151A11C2D6F4CD8A44077A850541CF4F18E158AD3E7D9290754CB79C4136A83</t>
+  </si>
+  <si>
+    <t>45E71AD4DC7771087F13887ECD6E004B5955A764F5842D7506C373CA740C603B</t>
+  </si>
+  <si>
+    <t>71FC7E1AF2F4E027C25709C95F986B53A728B21D1644F14ECFF3CB19914C252A</t>
+  </si>
+  <si>
+    <t>F2CFF2BD0FD4F1D6F28A8C331DFA7510EFA1606F7986F2F4A5B3CF2AB781F38A</t>
+  </si>
+  <si>
+    <t>7104E501BF2736D5FD4E447AD1927F6D95242BC55057D2C3A2DCB22F5725EABE</t>
+  </si>
+  <si>
+    <t>AA7C92583224AAA65B1199C941AEFB9430344422F914E6BEDE73670FFE5906AD</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>D9F090399C4C3C1976655A0915C762DC8AE04338DD665B3189F7A93935017E05</t>
+  </si>
+  <si>
+    <t>E5FFAA9903C6A3CF6FCF9CD17E84B85991E6D63A0F4606B3FF776E39728C9CF6</t>
+  </si>
+  <si>
+    <t>E8DFE1D0C000ED5E51794085819E56A998FBDF6357DD1032E886C4787D6E00E2</t>
+  </si>
+  <si>
+    <t>D1626A94D786553B2F1131985C61AAA3634647AF9E04016CB5DECA36B05EA3F1</t>
+  </si>
+  <si>
+    <t>F46ED237CF84CF7F2A773973AD12125E7E55B8C3251629ED2A53E9D1585698DE</t>
+  </si>
+  <si>
+    <t>AA9484CBAF43F22AF71B5AC76E10313B4213AFDC08CCEEB06733A0D5DCFEE756</t>
+  </si>
+  <si>
+    <t>F28B46AFDBE8BAE2F83553A4BCDF3E8E5127CAD0D0ACE66FD39788BA2EC11FFE</t>
+  </si>
+  <si>
+    <t>20D24518018576E6BAEC5CFF0A61152B28409FC4B2E996823C9E0A692016B5D0</t>
+  </si>
+  <si>
+    <t>5EC690E449D57A5978F0AF6DAD2491FBA215365338FC152736FF9D9884B4D48B</t>
+  </si>
+  <si>
+    <t>606812EF34EC662A132B43C6878A5D448E6D9D468BC6F5FEE46DD649F0BAF405</t>
+  </si>
+  <si>
+    <t>F28B4E311A6C2FC7B567306A81D43CFE8DC93F3AEEE97FAA2F7734B463A46881</t>
+  </si>
+  <si>
+    <t>E22467D5EFCD336DC9D7234A73A94D78E02D98189E294AE38617BE97CE8CCF04</t>
+  </si>
+  <si>
+    <t>3A139DC8689B404FC1A384692558CF603D9049F1248F4A643685328DA1A4F58E</t>
+  </si>
+  <si>
+    <t>2A5BD923FA14F9E20FB0D152DF2028A05EC2187369E93CCEFC672BFECD407AA5</t>
+  </si>
+  <si>
+    <t>04B5F8B1FDB6FE96ED0A9231D88877DDA55DA038F060F50F97F2406C465434DA</t>
+  </si>
+  <si>
+    <t>1D2587A898F72154AB82E97651CC17C0C2BCD0DAB97220CE16B47A0747FE813E</t>
+  </si>
+  <si>
+    <t>F68910DDD4A1E96B566C798C53422A1A2CC195F69BD47DCC87506A29828B51C2</t>
+  </si>
+  <si>
+    <t>F6E9E0FE8E1FF40A6B605217D2DE8C4D0D9B1C994F107EDCD18ABE0B22B2E8A4</t>
+  </si>
+  <si>
+    <t>EE16FB40FAA36B9007E8B39ACA2B27E377CAF2D708CBA8A595D967168D2CFEFE</t>
+  </si>
+  <si>
+    <t>778C544A70728E1243F423D69A6C1F88704B27A46610C39FF315FB23F40B7862</t>
+  </si>
+  <si>
+    <t>D0F0118ECAA72B30E6A963AE3DBDA5D4DEAB41880117ABB85623EE93C5731635</t>
+  </si>
+  <si>
+    <t>5209F42F76EDB3DF7DFB45B1D70F1FB6001DAB8BA38FD4D5E8C24134B6022A75</t>
+  </si>
+  <si>
+    <t>4B4B8398DFC8A9F3988766A24DAAC58992DA4C6282770A2139637154069A5A34</t>
+  </si>
+  <si>
+    <t>039CC48CD9F2D206A1128E0E8ACFB0F665367BE0696EF903F7485A840793C5B8</t>
+  </si>
+  <si>
+    <t>16B9218E334768FE24E8512A327FFF165CCB8FA93D23A1C68740D706E2E317B2</t>
+  </si>
+  <si>
+    <t>673003CC81E984BF572631455D674988CDDD7166F27692C331C4F8B6F92AAB5A</t>
+  </si>
+  <si>
+    <t>57487CFE9766192CE2DF0A186C0B630D52454A4B6CF7F42515E09F4BDD6EC4A4</t>
+  </si>
+  <si>
+    <t>A4133D0015A06A0EC496E4711AAA6AA59E58CF8E5AD21281AC8EA33E869BC47A</t>
+  </si>
+  <si>
+    <t>354B3A4B4836F7BB9A11F854155B8AB996A6692361FC04F71EC4C855EA970D20</t>
+  </si>
+  <si>
+    <t>5C82631B2063B2AEF671650317AF262A70AC7AD4158A0D31157159E00CBE6D70</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +355,27 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
     </font>
   </fonts>
   <fills count="4">
@@ -255,10 +427,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -274,9 +447,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{5FEA38D1-7748-4037-BD03-E5D112E423DE}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -582,7 +761,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,54 +778,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -661,7 +840,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -671,33 +852,558 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -707,33 +1413,75 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+      <c r="A2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -743,476 +1491,59 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+      <c r="A3" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A4" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1242,12 +1573,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1262,7 +1593,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1278,12 +1609,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1298,7 +1629,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1312,12 +1645,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1332,7 +1665,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1346,12 +1681,45 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F69480-3246-4E96-96D3-3BBE5DC16CCB}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1381,32 +1749,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1438,27 +1806,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1489,27 +1857,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1540,27 +1908,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1592,27 +1960,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1627,7 +1995,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1637,18 +2007,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+      <c r="A2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1663,7 +2033,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1673,18 +2045,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>